<commit_message>
USD Market and SynthQuotesFeed Refresh
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YC1YBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YC1YBootstrapping.xlsx
@@ -2775,7 +2775,7 @@
         <v>80</v>
       </c>
       <c r="D12" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D14" s="18" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYC1Y#0014</v>
+        <v>_USDYC1Y#0002</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -3383,7 +3383,7 @@
       <c r="B27" s="7"/>
       <c r="C27" s="30">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="D27" s="31">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -3424,11 +3424,11 @@
       <c r="B28" s="7"/>
       <c r="C28" s="32">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>60044</v>
+        <v>60062</v>
       </c>
       <c r="D28" s="11">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.16148492931212496</v>
+        <v>0.15470296919705304</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -5056,7 +5056,7 @@
       </c>
       <c r="F4" s="87">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>5.0559999999999997E-3</v>
+        <v>5.0359999999999997E-3</v>
       </c>
       <c r="G4" s="87"/>
       <c r="H4" s="88" t="b">
@@ -5070,11 +5070,11 @@
       </c>
       <c r="K4" s="78">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L4" s="89">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41782</v>
+        <v>41800</v>
       </c>
       <c r="M4" s="60">
         <v>30</v>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="F5" s="87">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>5.0559999999999997E-3</v>
+        <v>5.0359999999999997E-3</v>
       </c>
       <c r="G5" s="87"/>
       <c r="H5" s="88" t="b">
@@ -5109,11 +5109,11 @@
       </c>
       <c r="K5" s="78">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L5" s="89">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41788</v>
+        <v>41806</v>
       </c>
       <c r="M5" s="60">
         <v>40</v>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="F6" s="87">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>5.0559999999999997E-3</v>
+        <v>5.0359999999999997E-3</v>
       </c>
       <c r="G6" s="87"/>
       <c r="H6" s="88" t="b">
@@ -5148,11 +5148,11 @@
       </c>
       <c r="K6" s="78">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L6" s="89">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41795</v>
+        <v>41813</v>
       </c>
       <c r="M6" s="60">
         <v>50</v>
@@ -5173,7 +5173,7 @@
       </c>
       <c r="F7" s="87">
         <f>_xll.qlRateHelperQuoteValue($E7,Trigger)</f>
-        <v>5.0559999999999997E-3</v>
+        <v>5.0359999999999997E-3</v>
       </c>
       <c r="G7" s="87"/>
       <c r="H7" s="88" t="b">
@@ -5187,11 +5187,11 @@
       </c>
       <c r="K7" s="78">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L7" s="89">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41802</v>
+        <v>41820</v>
       </c>
       <c r="M7" s="60">
         <v>60</v>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="F8" s="87">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
-        <v>5.0460000000000001E-3</v>
+        <v>5.0260000000000001E-3</v>
       </c>
       <c r="G8" s="87"/>
       <c r="H8" s="88" t="b">
@@ -5226,11 +5226,11 @@
       </c>
       <c r="K8" s="78">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L8" s="89">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41813</v>
+        <v>41829</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="F9" s="87">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
-        <v>5.0460000000000001E-3</v>
+        <v>5.0260000000000001E-3</v>
       </c>
       <c r="G9" s="87"/>
       <c r="H9" s="88" t="b">
@@ -5259,11 +5259,11 @@
       </c>
       <c r="K9" s="78">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L9" s="89">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>41842</v>
+        <v>41862</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="F10" s="87">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
-        <v>5.0660000000000002E-3</v>
+        <v>5.0359999999999997E-3</v>
       </c>
       <c r="G10" s="87"/>
       <c r="H10" s="88" t="b">
@@ -5292,11 +5292,11 @@
       </c>
       <c r="K10" s="78">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L10" s="89">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
-        <v>41873</v>
+        <v>41891</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -5311,7 +5311,7 @@
       </c>
       <c r="F11" s="87">
         <f>_xll.qlRateHelperQuoteValue($E11,Trigger)</f>
-        <v>5.0759999999999998E-3</v>
+        <v>5.0559999999999997E-3</v>
       </c>
       <c r="G11" s="87"/>
       <c r="H11" s="88" t="b">
@@ -5325,11 +5325,11 @@
       </c>
       <c r="K11" s="78">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L11" s="89">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>41904</v>
+        <v>41921</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -5344,7 +5344,7 @@
       </c>
       <c r="F12" s="87">
         <f>_xll.qlRateHelperQuoteValue($E12,Trigger)</f>
-        <v>5.0860000000000002E-3</v>
+        <v>5.0660000000000002E-3</v>
       </c>
       <c r="G12" s="87"/>
       <c r="H12" s="88" t="b">
@@ -5358,11 +5358,11 @@
       </c>
       <c r="K12" s="78">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L12" s="89">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>41934</v>
+        <v>41953</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="F13" s="87">
         <f>_xll.qlRateHelperQuoteValue($E13,Trigger)</f>
-        <v>5.1060000000000003E-3</v>
+        <v>5.0860000000000002E-3</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="88" t="b">
@@ -5391,11 +5391,11 @@
       </c>
       <c r="K13" s="78">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L13" s="89">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
-        <v>41967</v>
+        <v>41982</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -5410,7 +5410,7 @@
       </c>
       <c r="F14" s="87">
         <f>_xll.qlRateHelperQuoteValue($E14,Trigger)</f>
-        <v>5.1859999999999996E-3</v>
+        <v>5.176E-3</v>
       </c>
       <c r="G14" s="87"/>
       <c r="H14" s="88" t="b">
@@ -5424,11 +5424,11 @@
       </c>
       <c r="K14" s="78">
         <f>_xll.qlRateHelperEarliestDate($E14,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L14" s="89">
         <f>_xll.qlRateHelperLatestDate($E14,Trigger)</f>
-        <v>42058</v>
+        <v>42072</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -5457,11 +5457,11 @@
       </c>
       <c r="K15" s="95">
         <f>_xll.qlRateHelperEarliestDate($E15,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L15" s="96">
         <f>_xll.qlRateHelperLatestDate($E15,Trigger)</f>
-        <v>42146</v>
+        <v>42164</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="F16" s="87">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
-        <v>5.4499999999999991E-3</v>
+        <v>5.4699999999999992E-3</v>
       </c>
       <c r="G16" s="87"/>
       <c r="H16" s="88" t="b">
@@ -5495,11 +5495,11 @@
       </c>
       <c r="K16" s="78">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>41813</v>
+        <v>41829</v>
       </c>
       <c r="L16" s="89">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>42178</v>
+        <v>42194</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="F17" s="87">
         <f>_xll.qlRateHelperQuoteValue($E17,Trigger)</f>
-        <v>5.6099999999999995E-3</v>
+        <v>5.7099999999999998E-3</v>
       </c>
       <c r="G17" s="87"/>
       <c r="H17" s="88" t="b">
@@ -5533,11 +5533,11 @@
       </c>
       <c r="K17" s="78">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>41842</v>
+        <v>41862</v>
       </c>
       <c r="L17" s="89">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>42207</v>
+        <v>42227</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="F18" s="87">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>5.8200000000000005E-3</v>
+        <v>5.9699999999999996E-3</v>
       </c>
       <c r="G18" s="87"/>
       <c r="H18" s="88" t="b">
@@ -5571,11 +5571,11 @@
       </c>
       <c r="K18" s="78">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>41873</v>
+        <v>41891</v>
       </c>
       <c r="L18" s="89">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>42240</v>
+        <v>42256</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -5595,7 +5595,7 @@
       </c>
       <c r="F19" s="87">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>6.0799999999999995E-3</v>
+        <v>6.2700000000000004E-3</v>
       </c>
       <c r="G19" s="87"/>
       <c r="H19" s="88" t="b">
@@ -5609,11 +5609,11 @@
       </c>
       <c r="K19" s="78">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>41904</v>
+        <v>41921</v>
       </c>
       <c r="L19" s="89">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>42269</v>
+        <v>42286</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="F20" s="87">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>6.3899999999999998E-3</v>
+        <v>6.6400000000000001E-3</v>
       </c>
       <c r="G20" s="87"/>
       <c r="H20" s="88" t="b">
@@ -5647,11 +5647,11 @@
       </c>
       <c r="K20" s="78">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>41934</v>
+        <v>41953</v>
       </c>
       <c r="L20" s="89">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>42299</v>
+        <v>42318</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="F21" s="87">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>6.7799999999999996E-3</v>
+        <v>7.0500000000000007E-3</v>
       </c>
       <c r="G21" s="87"/>
       <c r="H21" s="88" t="b">
@@ -5685,11 +5685,11 @@
       </c>
       <c r="K21" s="78">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>41967</v>
+        <v>41982</v>
       </c>
       <c r="L21" s="89">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>42332</v>
+        <v>42347</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="F22" s="87">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>7.1349999999999998E-3</v>
+        <v>7.221E-3</v>
       </c>
       <c r="G22" s="87"/>
       <c r="H22" s="88" t="b">
@@ -5723,11 +5723,11 @@
       </c>
       <c r="K22" s="78">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>41995</v>
+        <v>42013</v>
       </c>
       <c r="L22" s="89">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>42360</v>
+        <v>42380</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="F23" s="87">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>7.646E-3</v>
+        <v>7.6819999999999996E-3</v>
       </c>
       <c r="G23" s="87"/>
       <c r="H23" s="88" t="b">
@@ -5761,11 +5761,11 @@
       </c>
       <c r="K23" s="78">
         <f>_xll.qlRateHelperEarliestDate($E23,Trigger)</f>
-        <v>42026</v>
+        <v>42044</v>
       </c>
       <c r="L23" s="89">
         <f>_xll.qlRateHelperLatestDate($E23,Trigger)</f>
-        <v>42391</v>
+        <v>42409</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="F24" s="87">
         <f>_xll.qlRateHelperQuoteValue($E24,Trigger)</f>
-        <v>8.2199999999999999E-3</v>
+        <v>8.6199999999999992E-3</v>
       </c>
       <c r="G24" s="87"/>
       <c r="H24" s="88" t="b">
@@ -5799,11 +5799,11 @@
       </c>
       <c r="K24" s="78">
         <f>_xll.qlRateHelperEarliestDate($E24,Trigger)</f>
-        <v>42058</v>
+        <v>42072</v>
       </c>
       <c r="L24" s="89">
         <f>_xll.qlRateHelperLatestDate($E24,Trigger)</f>
-        <v>42423</v>
+        <v>42438</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
@@ -5823,7 +5823,7 @@
       </c>
       <c r="F25" s="87">
         <f>_xll.qlRateHelperQuoteValue($E25,Trigger)</f>
-        <v>8.7779999999999993E-3</v>
+        <v>8.7749999999999998E-3</v>
       </c>
       <c r="G25" s="87"/>
       <c r="H25" s="88" t="b">
@@ -5837,11 +5837,11 @@
       </c>
       <c r="K25" s="78">
         <f>_xll.qlRateHelperEarliestDate($E25,Trigger)</f>
-        <v>42086</v>
+        <v>42103</v>
       </c>
       <c r="L25" s="89">
         <f>_xll.qlRateHelperLatestDate($E25,Trigger)</f>
-        <v>42452</v>
+        <v>42471</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="F26" s="87">
         <f>_xll.qlRateHelperQuoteValue($E26,Trigger)</f>
-        <v>9.4219999999999998E-3</v>
+        <v>9.3749999999999997E-3</v>
       </c>
       <c r="G26" s="87"/>
       <c r="H26" s="88" t="b">
@@ -5875,11 +5875,11 @@
       </c>
       <c r="K26" s="78">
         <f>_xll.qlRateHelperEarliestDate($E26,Trigger)</f>
-        <v>42116</v>
+        <v>42135</v>
       </c>
       <c r="L26" s="89">
         <f>_xll.qlRateHelperLatestDate($E26,Trigger)</f>
-        <v>42482</v>
+        <v>42501</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -5899,7 +5899,7 @@
       </c>
       <c r="F27" s="87">
         <f>_xll.qlRateHelperQuoteValue($E27,Trigger)</f>
-        <v>1.008E-2</v>
+        <v>1.0669999999999999E-2</v>
       </c>
       <c r="G27" s="87"/>
       <c r="H27" s="88" t="b">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="K27" s="78">
         <f>_xll.qlRateHelperEarliestDate($E27,Trigger)</f>
-        <v>42146</v>
+        <v>42164</v>
       </c>
       <c r="L27" s="89">
         <f>_xll.qlRateHelperLatestDate($E27,Trigger)</f>
-        <v>42513</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="F28" s="87">
         <f>_xll.qlRateHelperQuoteValue($E28,Trigger)</f>
-        <v>1.0770999999999999E-2</v>
+        <v>1.0761E-2</v>
       </c>
       <c r="G28" s="87"/>
       <c r="H28" s="88" t="b">
@@ -5951,11 +5951,11 @@
       </c>
       <c r="K28" s="78">
         <f>_xll.qlRateHelperEarliestDate($E28,Trigger)</f>
-        <v>42177</v>
+        <v>42194</v>
       </c>
       <c r="L28" s="89">
         <f>_xll.qlRateHelperLatestDate($E28,Trigger)</f>
-        <v>42543</v>
+        <v>42562</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
@@ -5975,7 +5975,7 @@
       </c>
       <c r="F29" s="87">
         <f>_xll.qlRateHelperQuoteValue($E29,Trigger)</f>
-        <v>1.1464E-2</v>
+        <v>1.1455E-2</v>
       </c>
       <c r="G29" s="87"/>
       <c r="H29" s="88" t="b">
@@ -5989,11 +5989,11 @@
       </c>
       <c r="K29" s="78">
         <f>_xll.qlRateHelperEarliestDate($E29,Trigger)</f>
-        <v>42207</v>
+        <v>42226</v>
       </c>
       <c r="L29" s="89">
         <f>_xll.qlRateHelperLatestDate($E29,Trigger)</f>
-        <v>42573</v>
+        <v>42592</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="F30" s="87">
         <f>_xll.qlRateHelperQuoteValue($E30,Trigger)</f>
-        <v>1.2241E-2</v>
+        <v>1.2232E-2</v>
       </c>
       <c r="G30" s="87"/>
       <c r="H30" s="88" t="b">
@@ -6027,11 +6027,11 @@
       </c>
       <c r="K30" s="78">
         <f>_xll.qlRateHelperEarliestDate($E30,Trigger)</f>
-        <v>42240</v>
+        <v>42256</v>
       </c>
       <c r="L30" s="89">
         <f>_xll.qlRateHelperLatestDate($E30,Trigger)</f>
-        <v>42606</v>
+        <v>42622</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
@@ -6051,7 +6051,7 @@
       </c>
       <c r="F31" s="87">
         <f>_xll.qlRateHelperQuoteValue($E31,Trigger)</f>
-        <v>1.2952999999999999E-2</v>
+        <v>1.3017000000000001E-2</v>
       </c>
       <c r="G31" s="87"/>
       <c r="H31" s="88" t="b">
@@ -6065,11 +6065,11 @@
       </c>
       <c r="K31" s="78">
         <f>_xll.qlRateHelperEarliestDate($E31,Trigger)</f>
-        <v>42269</v>
+        <v>42286</v>
       </c>
       <c r="L31" s="89">
         <f>_xll.qlRateHelperLatestDate($E31,Trigger)</f>
-        <v>42635</v>
+        <v>42654</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="F32" s="87">
         <f>_xll.qlRateHelperQuoteValue($E32,Trigger)</f>
-        <v>1.3748E-2</v>
+        <v>1.3809E-2</v>
       </c>
       <c r="G32" s="87"/>
       <c r="H32" s="88" t="b">
@@ -6103,11 +6103,11 @@
       </c>
       <c r="K32" s="78">
         <f>_xll.qlRateHelperEarliestDate($E32,Trigger)</f>
-        <v>42299</v>
+        <v>42317</v>
       </c>
       <c r="L32" s="89">
         <f>_xll.qlRateHelperLatestDate($E32,Trigger)</f>
-        <v>42667</v>
+        <v>42683</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -6127,7 +6127,7 @@
       </c>
       <c r="F33" s="93">
         <f>_xll.qlRateHelperQuoteValue($E33,Trigger)</f>
-        <v>1.4519000000000001E-2</v>
+        <v>1.4671999999999999E-2</v>
       </c>
       <c r="G33" s="93"/>
       <c r="H33" s="94" t="b">
@@ -6141,11 +6141,11 @@
       </c>
       <c r="K33" s="95">
         <f>_xll.qlRateHelperEarliestDate($E33,Trigger)</f>
-        <v>42331</v>
+        <v>42347</v>
       </c>
       <c r="L33" s="96">
         <f>_xll.qlRateHelperLatestDate($E33,Trigger)</f>
-        <v>42697</v>
+        <v>42713</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6159,11 +6159,11 @@
       </c>
       <c r="D34" s="86" t="str">
         <f t="array" ref="D34:D75">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A34:$A75)</f>
-        <v>K4</v>
+        <v>M4</v>
       </c>
       <c r="E34" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YK4</v>
+        <v>USD_YC1YRH_FUT1YM4</v>
       </c>
       <c r="F34" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E34,Trigger)</f>
@@ -6201,11 +6201,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D35" s="86" t="str">
-        <v>M4</v>
+        <v>N4</v>
       </c>
       <c r="E35" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YM4</v>
+        <v>USD_YC1YRH_FUT1YN4</v>
       </c>
       <c r="F35" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
@@ -6243,11 +6243,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D36" s="86" t="str">
-        <v>N4</v>
+        <v>Q4</v>
       </c>
       <c r="E36" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YN4</v>
+        <v>USD_YC1YRH_FUT1YQ4</v>
       </c>
       <c r="F36" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -6285,11 +6285,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D37" s="86" t="str">
-        <v>Q4</v>
+        <v>U4</v>
       </c>
       <c r="E37" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YQ4</v>
+        <v>USD_YC1YRH_FUT1YU4</v>
       </c>
       <c r="F37" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -6327,11 +6327,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D38" s="86" t="str">
-        <v>U4</v>
+        <v>V4</v>
       </c>
       <c r="E38" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YU4</v>
+        <v>USD_YC1YRH_FUT1YV4</v>
       </c>
       <c r="F38" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -6369,11 +6369,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D39" s="86" t="str">
-        <v>V4</v>
+        <v>X4</v>
       </c>
       <c r="E39" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YV4</v>
+        <v>USD_YC1YRH_FUT1YX4</v>
       </c>
       <c r="F39" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -6411,11 +6411,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D40" s="86" t="str">
-        <v>X4</v>
+        <v>Z4</v>
       </c>
       <c r="E40" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YX4</v>
+        <v>USD_YC1YRH_FUT1YZ4</v>
       </c>
       <c r="F40" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -6453,11 +6453,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D41" s="86" t="str">
-        <v>Z4</v>
+        <v>F5</v>
       </c>
       <c r="E41" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YZ4</v>
+        <v>USD_YC1YRH_FUT1YF5</v>
       </c>
       <c r="F41" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -6495,11 +6495,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D42" s="86" t="str">
-        <v>F5</v>
+        <v>G5</v>
       </c>
       <c r="E42" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YF5</v>
+        <v>USD_YC1YRH_FUT1YG5</v>
       </c>
       <c r="F42" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -6537,11 +6537,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D43" s="86" t="str">
-        <v>G5</v>
+        <v>H5</v>
       </c>
       <c r="E43" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YG5</v>
+        <v>USD_YC1YRH_FUT1YH5</v>
       </c>
       <c r="F43" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -6579,11 +6579,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D44" s="86" t="str">
-        <v>H5</v>
+        <v>J5</v>
       </c>
       <c r="E44" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YH5</v>
+        <v>USD_YC1YRH_FUT1YJ5</v>
       </c>
       <c r="F44" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -6621,11 +6621,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D45" s="86" t="str">
-        <v>J5</v>
+        <v>K5</v>
       </c>
       <c r="E45" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>USD_YC1YRH_FUT1YJ5</v>
+        <v>USD_YC1YRH_FUT1YK5</v>
       </c>
       <c r="F45" s="100" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -10209,7 +10209,7 @@
       </c>
       <c r="F131" s="87">
         <f>_xll.qlRateHelperQuoteValue($E131,Trigger)</f>
-        <v>5.3416500339135012E-3</v>
+        <v>5.3472838322122735E-3</v>
       </c>
       <c r="G131" s="87">
         <f>_xll.qlSwapRateHelperSpread($E131,Trigger)</f>
@@ -10226,11 +10226,11 @@
       </c>
       <c r="K131" s="78">
         <f>_xll.qlRateHelperEarliestDate($E131,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L131" s="89">
         <f>_xll.qlRateHelperLatestDate($E131,Trigger)</f>
-        <v>42146</v>
+        <v>42164</v>
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.25">
@@ -10377,7 +10377,7 @@
       </c>
       <c r="F135" s="87">
         <f>_xll.qlRateHelperQuoteValue($E135,Trigger)</f>
-        <v>7.754693010562118E-3</v>
+        <v>7.9799585295124899E-3</v>
       </c>
       <c r="G135" s="87">
         <f>_xll.qlSwapRateHelperSpread($E135,Trigger)</f>
@@ -10394,11 +10394,11 @@
       </c>
       <c r="K135" s="78">
         <f>_xll.qlRateHelperEarliestDate($E135,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L135" s="89">
         <f>_xll.qlRateHelperLatestDate($E135,Trigger)</f>
-        <v>42513</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.25">
@@ -10419,7 +10419,7 @@
       </c>
       <c r="F136" s="87">
         <f>_xll.qlRateHelperQuoteValue($E136,Trigger)</f>
-        <v>1.164901613355118E-2</v>
+        <v>1.2019217681891072E-2</v>
       </c>
       <c r="G136" s="87">
         <f>_xll.qlSwapRateHelperSpread($E136,Trigger)</f>
@@ -10436,11 +10436,11 @@
       </c>
       <c r="K136" s="78">
         <f>_xll.qlRateHelperEarliestDate($E136,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L136" s="89">
         <f>_xll.qlRateHelperLatestDate($E136,Trigger)</f>
-        <v>42877</v>
+        <v>42895</v>
       </c>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.25">
@@ -10461,7 +10461,7 @@
       </c>
       <c r="F137" s="87">
         <f>_xll.qlRateHelperQuoteValue($E137,Trigger)</f>
-        <v>1.5532928591970138E-2</v>
+        <v>1.6133293309975427E-2</v>
       </c>
       <c r="G137" s="87">
         <f>_xll.qlSwapRateHelperSpread($E137,Trigger)</f>
@@ -10478,11 +10478,11 @@
       </c>
       <c r="K137" s="78">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L137" s="89">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>43242</v>
+        <v>43262</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.25">
@@ -10503,7 +10503,7 @@
       </c>
       <c r="F138" s="87">
         <f>_xll.qlRateHelperQuoteValue($E138,Trigger)</f>
-        <v>1.8856057589906713E-2</v>
+        <v>1.9626592515768052E-2</v>
       </c>
       <c r="G138" s="87">
         <f>_xll.qlSwapRateHelperSpread($E138,Trigger)</f>
@@ -10520,11 +10520,11 @@
       </c>
       <c r="K138" s="78">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L138" s="89">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>43607</v>
+        <v>43626</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.25">
@@ -10545,7 +10545,7 @@
       </c>
       <c r="F139" s="87">
         <f>_xll.qlRateHelperQuoteValue($E139,Trigger)</f>
-        <v>2.1648616902011295E-2</v>
+        <v>2.2489103454696721E-2</v>
       </c>
       <c r="G139" s="87">
         <f>_xll.qlSwapRateHelperSpread($E139,Trigger)</f>
@@ -10562,11 +10562,11 @@
       </c>
       <c r="K139" s="78">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L139" s="89">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
-        <v>43973</v>
+        <v>43991</v>
       </c>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.25">
@@ -10587,7 +10587,7 @@
       </c>
       <c r="F140" s="87">
         <f>_xll.qlRateHelperQuoteValue($E140,Trigger)</f>
-        <v>2.3930540650813428E-2</v>
+        <v>2.4811040117459097E-2</v>
       </c>
       <c r="G140" s="87">
         <f>_xll.qlSwapRateHelperSpread($E140,Trigger)</f>
@@ -10604,11 +10604,11 @@
       </c>
       <c r="K140" s="78">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L140" s="89">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
-        <v>44340</v>
+        <v>44356</v>
       </c>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.25">
@@ -10629,7 +10629,7 @@
       </c>
       <c r="F141" s="87">
         <f>_xll.qlRateHelperQuoteValue($E141,Trigger)</f>
-        <v>2.5801991147985238E-2</v>
+        <v>2.6682497469501069E-2</v>
       </c>
       <c r="G141" s="87">
         <f>_xll.qlSwapRateHelperSpread($E141,Trigger)</f>
@@ -10646,11 +10646,11 @@
       </c>
       <c r="K141" s="78">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L141" s="89">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>44704</v>
+        <v>44721</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.25">
@@ -10671,7 +10671,7 @@
       </c>
       <c r="F142" s="87">
         <f>_xll.qlRateHelperQuoteValue($E142,Trigger)</f>
-        <v>2.7353168245615473E-2</v>
+        <v>2.8223635133069854E-2</v>
       </c>
       <c r="G142" s="87">
         <f>_xll.qlSwapRateHelperSpread($E142,Trigger)</f>
@@ -10688,11 +10688,11 @@
       </c>
       <c r="K142" s="78">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L142" s="89">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>45068</v>
+        <v>45086</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.25">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="F143" s="87">
         <f>_xll.qlRateHelperQuoteValue($E143,Trigger)</f>
-        <v>2.8664063485976134E-2</v>
+        <v>2.9524682111459762E-2</v>
       </c>
       <c r="G143" s="87">
         <f>_xll.qlSwapRateHelperSpread($E143,Trigger)</f>
@@ -10730,11 +10730,11 @@
       </c>
       <c r="K143" s="78">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L143" s="89">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>45434</v>
+        <v>45453</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.25">
@@ -10755,7 +10755,7 @@
       </c>
       <c r="F144" s="87">
         <f>_xll.qlRateHelperQuoteValue($E144,Trigger)</f>
-        <v>2.9774794829145777E-2</v>
+        <v>3.0634087424217363E-2</v>
       </c>
       <c r="G144" s="87">
         <f>_xll.qlSwapRateHelperSpread($E144,Trigger)</f>
@@ -10772,11 +10772,11 @@
       </c>
       <c r="K144" s="78">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L144" s="89">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>45799</v>
+        <v>45817</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.25">
@@ -10797,7 +10797,7 @@
       </c>
       <c r="F145" s="87">
         <f>_xll.qlRateHelperQuoteValue($E145,Trigger)</f>
-        <v>3.0715617484556201E-2</v>
+        <v>3.1586118645384104E-2</v>
       </c>
       <c r="G145" s="87">
         <f>_xll.qlSwapRateHelperSpread($E145,Trigger)</f>
@@ -10814,11 +10814,11 @@
       </c>
       <c r="K145" s="78">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L145" s="89">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
-        <v>46164</v>
+        <v>46182</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
       </c>
       <c r="F146" s="87">
         <f>_xll.qlRateHelperQuoteValue($E146,Trigger)</f>
-        <v>3.1510209893080628E-2</v>
+        <v>3.2389756231615809E-2</v>
       </c>
       <c r="G146" s="87">
         <f>_xll.qlSwapRateHelperSpread($E146,Trigger)</f>
@@ -10856,11 +10856,11 @@
       </c>
       <c r="K146" s="78">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L146" s="89">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>46531</v>
+        <v>46547</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.25">
@@ -10881,7 +10881,7 @@
       </c>
       <c r="F147" s="87">
         <f>_xll.qlRateHelperQuoteValue($E147,Trigger)</f>
-        <v>3.2173611587713299E-2</v>
+        <v>3.3070237561938255E-2</v>
       </c>
       <c r="G147" s="87">
         <f>_xll.qlSwapRateHelperSpread($E147,Trigger)</f>
@@ -10898,11 +10898,11 @@
       </c>
       <c r="K147" s="78">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L147" s="89">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>46895</v>
+        <v>46913</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.25">
@@ -10923,7 +10923,7 @@
       </c>
       <c r="F148" s="87">
         <f>_xll.qlRateHelperQuoteValue($E148,Trigger)</f>
-        <v>3.273691034385539E-2</v>
+        <v>3.3647436284933101E-2</v>
       </c>
       <c r="G148" s="87">
         <f>_xll.qlSwapRateHelperSpread($E148,Trigger)</f>
@@ -10940,11 +10940,11 @@
       </c>
       <c r="K148" s="78">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L148" s="89">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>47260</v>
+        <v>47280</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.25">
@@ -10965,7 +10965,7 @@
       </c>
       <c r="F149" s="87">
         <f>_xll.qlRateHelperQuoteValue($E149,Trigger)</f>
-        <v>3.3215321781516129E-2</v>
+        <v>3.4131830610649241E-2</v>
       </c>
       <c r="G149" s="87">
         <f>_xll.qlSwapRateHelperSpread($E149,Trigger)</f>
@@ -10982,11 +10982,11 @@
       </c>
       <c r="K149" s="78">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L149" s="89">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>47625</v>
+        <v>47644</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
       </c>
       <c r="F150" s="87">
         <f>_xll.qlRateHelperQuoteValue($E150,Trigger)</f>
-        <v>3.3623377590231963E-2</v>
+        <v>3.4543485190088367E-2</v>
       </c>
       <c r="G150" s="87">
         <f>_xll.qlSwapRateHelperSpread($E150,Trigger)</f>
@@ -11024,11 +11024,11 @@
       </c>
       <c r="K150" s="78">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L150" s="89">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
-        <v>47990</v>
+        <v>48008</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.25">
@@ -11049,7 +11049,7 @@
       </c>
       <c r="F151" s="87">
         <f>_xll.qlRateHelperQuoteValue($E151,Trigger)</f>
-        <v>3.3975416680370026E-2</v>
+        <v>3.4895962246259953E-2</v>
       </c>
       <c r="G151" s="87">
         <f>_xll.qlSwapRateHelperSpread($E151,Trigger)</f>
@@ -11066,11 +11066,11 @@
       </c>
       <c r="K151" s="78">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L151" s="89">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
-        <v>48358</v>
+        <v>48374</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.25">
@@ -11091,7 +11091,7 @@
       </c>
       <c r="F152" s="87">
         <f>_xll.qlRateHelperQuoteValue($E152,Trigger)</f>
-        <v>3.4273208222611193E-2</v>
+        <v>3.5194901989380051E-2</v>
       </c>
       <c r="G152" s="87">
         <f>_xll.qlSwapRateHelperSpread($E152,Trigger)</f>
@@ -11108,11 +11108,11 @@
       </c>
       <c r="K152" s="78">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L152" s="89">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>48722</v>
+        <v>48739</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.25">
@@ -11133,7 +11133,7 @@
       </c>
       <c r="F153" s="87">
         <f>_xll.qlRateHelperQuoteValue($E153,Trigger)</f>
-        <v>3.452808326448225E-2</v>
+        <v>3.5448540914528488E-2</v>
       </c>
       <c r="G153" s="87">
         <f>_xll.qlSwapRateHelperSpread($E153,Trigger)</f>
@@ -11150,11 +11150,11 @@
       </c>
       <c r="K153" s="78">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L153" s="89">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>49086</v>
+        <v>49104</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.25">
@@ -11175,7 +11175,7 @@
       </c>
       <c r="F154" s="87">
         <f>_xll.qlRateHelperQuoteValue($E154,Trigger)</f>
-        <v>3.4746334188534275E-2</v>
+        <v>3.5664077078164984E-2</v>
       </c>
       <c r="G154" s="87">
         <f>_xll.qlSwapRateHelperSpread($E154,Trigger)</f>
@@ -11192,11 +11192,11 @@
       </c>
       <c r="K154" s="78">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L154" s="89">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>49451</v>
+        <v>49471</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.25">
@@ -11217,7 +11217,7 @@
       </c>
       <c r="F155" s="87">
         <f>_xll.qlRateHelperQuoteValue($E155,Trigger)</f>
-        <v>3.4933385374086037E-2</v>
+        <v>3.5844525985518225E-2</v>
       </c>
       <c r="G155" s="87">
         <f>_xll.qlSwapRateHelperSpread($E155,Trigger)</f>
@@ -11234,11 +11234,11 @@
       </c>
       <c r="K155" s="78">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L155" s="89">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>49817</v>
+        <v>49835</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.25">
@@ -11259,7 +11259,7 @@
       </c>
       <c r="F156" s="87">
         <f>_xll.qlRateHelperQuoteValue($E156,Trigger)</f>
-        <v>3.5093059937820879E-2</v>
+        <v>3.5997869355324785E-2</v>
       </c>
       <c r="G156" s="87">
         <f>_xll.qlSwapRateHelperSpread($E156,Trigger)</f>
@@ -11276,11 +11276,11 @@
       </c>
       <c r="K156" s="78">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L156" s="89">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
-        <v>50182</v>
+        <v>50200</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.25">
@@ -11301,7 +11301,7 @@
       </c>
       <c r="F157" s="87">
         <f>_xll.qlRateHelperQuoteValue($E157,Trigger)</f>
-        <v>3.523094916792377E-2</v>
+        <v>3.612803369884502E-2</v>
       </c>
       <c r="G157" s="87">
         <f>_xll.qlSwapRateHelperSpread($E157,Trigger)</f>
@@ -11318,11 +11318,11 @@
       </c>
       <c r="K157" s="78">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L157" s="89">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
-        <v>50549</v>
+        <v>50565</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
       </c>
       <c r="F158" s="87">
         <f>_xll.qlRateHelperQuoteValue($E158,Trigger)</f>
-        <v>3.5348449501041962E-2</v>
+        <v>3.6238855439511539E-2</v>
       </c>
       <c r="G158" s="87">
         <f>_xll.qlSwapRateHelperSpread($E158,Trigger)</f>
@@ -11360,11 +11360,11 @@
       </c>
       <c r="K158" s="78">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L158" s="89">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>50913</v>
+        <v>50930</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.25">
@@ -11385,7 +11385,7 @@
       </c>
       <c r="F159" s="87">
         <f>_xll.qlRateHelperQuoteValue($E159,Trigger)</f>
-        <v>3.5450101555636104E-2</v>
+        <v>3.6334455694744423E-2</v>
       </c>
       <c r="G159" s="87">
         <f>_xll.qlSwapRateHelperSpread($E159,Trigger)</f>
@@ -11402,11 +11402,11 @@
       </c>
       <c r="K159" s="78">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L159" s="89">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>51278</v>
+        <v>51298</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.25">
@@ -11427,7 +11427,7 @@
       </c>
       <c r="F160" s="87">
         <f>_xll.qlRateHelperQuoteValue($E160,Trigger)</f>
-        <v>3.553746372544702E-2</v>
+        <v>3.6415412768812688E-2</v>
       </c>
       <c r="G160" s="87">
         <f>_xll.qlSwapRateHelperSpread($E160,Trigger)</f>
@@ -11444,11 +11444,11 @@
       </c>
       <c r="K160" s="78">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L160" s="89">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>51643</v>
+        <v>51662</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
@@ -11469,7 +11469,7 @@
       </c>
       <c r="F161" s="87">
         <f>_xll.qlRateHelperQuoteValue($E161,Trigger)</f>
-        <v>3.5612088463245505E-2</v>
+        <v>3.648525421632233E-2</v>
       </c>
       <c r="G161" s="87">
         <f>_xll.qlSwapRateHelperSpread($E161,Trigger)</f>
@@ -11486,11 +11486,11 @@
       </c>
       <c r="K161" s="78">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L161" s="89">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>52008</v>
+        <v>52026</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
@@ -11511,7 +11511,7 @@
       </c>
       <c r="F162" s="87">
         <f>_xll.qlRateHelperQuoteValue($E162,Trigger)</f>
-        <v>3.5675290060732202E-2</v>
+        <v>3.6545988690413075E-2</v>
       </c>
       <c r="G162" s="87">
         <f>_xll.qlSwapRateHelperSpread($E162,Trigger)</f>
@@ -11528,11 +11528,11 @@
       </c>
       <c r="K162" s="78">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L162" s="89">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
-        <v>52373</v>
+        <v>52391</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.25">
@@ -11553,7 +11553,7 @@
       </c>
       <c r="F163" s="87">
         <f>_xll.qlRateHelperQuoteValue($E163,Trigger)</f>
-        <v>3.5728530220437316E-2</v>
+        <v>3.6599057160298439E-2</v>
       </c>
       <c r="G163" s="87">
         <f>_xll.qlSwapRateHelperSpread($E163,Trigger)</f>
@@ -11570,11 +11570,11 @@
       </c>
       <c r="K163" s="78">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L163" s="89">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>52740</v>
+        <v>52757</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.25">
@@ -11595,7 +11595,7 @@
       </c>
       <c r="F164" s="87">
         <f>_xll.qlRateHelperQuoteValue($E164,Trigger)</f>
-        <v>3.5886758472093862E-2</v>
+        <v>3.6771807077715532E-2</v>
       </c>
       <c r="G164" s="87">
         <f>_xll.qlSwapRateHelperSpread($E164,Trigger)</f>
@@ -11612,11 +11612,11 @@
       </c>
       <c r="K164" s="78">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L164" s="89">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>54567</v>
+        <v>54583</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.25">
@@ -11637,7 +11637,7 @@
       </c>
       <c r="F165" s="87">
         <f>_xll.qlRateHelperQuoteValue($E165,Trigger)</f>
-        <v>3.5898674654738019E-2</v>
+        <v>3.67991537539194E-2</v>
       </c>
       <c r="G165" s="87">
         <f>_xll.qlSwapRateHelperSpread($E165,Trigger)</f>
@@ -11654,11 +11654,11 @@
       </c>
       <c r="K165" s="78">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L165" s="89">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>56391</v>
+        <v>56409</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
       </c>
       <c r="F166" s="87">
         <f>_xll.qlRateHelperQuoteValue($E166,Trigger)</f>
-        <v>3.572849704733444E-2</v>
+        <v>3.659896924229504E-2</v>
       </c>
       <c r="G166" s="87">
         <f>_xll.qlSwapRateHelperSpread($E166,Trigger)</f>
@@ -11696,11 +11696,11 @@
       </c>
       <c r="K166" s="78">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L166" s="89">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>60044</v>
+        <v>60062</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.25">
@@ -11721,7 +11721,7 @@
       </c>
       <c r="F167" s="93">
         <f>_xll.qlRateHelperQuoteValue($E167,Trigger)</f>
-        <v>3.5580491109318928E-2</v>
+        <v>3.6418638736905318E-2</v>
       </c>
       <c r="G167" s="93">
         <f>_xll.qlSwapRateHelperSpread($E167,Trigger)</f>
@@ -11738,11 +11738,11 @@
       </c>
       <c r="K167" s="95">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="L167" s="96">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>63696</v>
+        <v>63716</v>
       </c>
     </row>
   </sheetData>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="E2" s="68">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>5.0460000000000001E-3</v>
+        <v>5.0260000000000001E-3</v>
       </c>
       <c r="F2" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -11823,14 +11823,14 @@
       </c>
       <c r="G2" s="78">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H2" s="79">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41813</v>
+        <v>41829</v>
       </c>
       <c r="I2" s="64">
-        <v>0.99955166775862125</v>
+        <v>0.99958134201458615</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -11845,7 +11845,7 @@
       </c>
       <c r="E3" s="68">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>5.0460000000000001E-3</v>
+        <v>5.0260000000000001E-3</v>
       </c>
       <c r="F3" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -11853,14 +11853,14 @@
       </c>
       <c r="G3" s="78">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H3" s="79">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41842</v>
+        <v>41862</v>
       </c>
       <c r="I3" s="64">
-        <v>0.9991457137623071</v>
+        <v>0.99912122292837724</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -11875,7 +11875,7 @@
       </c>
       <c r="E4" s="68">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>5.0660000000000002E-3</v>
+        <v>5.0359999999999997E-3</v>
       </c>
       <c r="F4" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -11883,14 +11883,14 @@
       </c>
       <c r="G4" s="78">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H4" s="79">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41873</v>
+        <v>41891</v>
       </c>
       <c r="I4" s="64">
-        <v>0.99870702949248702</v>
+        <v>0.99871467640509581</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -11905,7 +11905,7 @@
       </c>
       <c r="E5" s="68">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>5.0759999999999998E-3</v>
+        <v>5.0559999999999997E-3</v>
       </c>
       <c r="F5" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -11913,14 +11913,14 @@
       </c>
       <c r="G5" s="78">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H5" s="79">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41904</v>
+        <v>41921</v>
       </c>
       <c r="I5" s="64">
-        <v>0.99826870258903944</v>
+        <v>0.99828950857204946</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -11936,7 +11936,7 @@
       </c>
       <c r="E6" s="68">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>5.0860000000000002E-3</v>
+        <v>5.0660000000000002E-3</v>
       </c>
       <c r="F6" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -11944,20 +11944,20 @@
       </c>
       <c r="G6" s="78">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H6" s="79">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41934</v>
+        <v>41953</v>
       </c>
       <c r="I6" s="64">
-        <v>0.99784311222069111</v>
+        <v>0.99783756404069934</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="73" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YC1YRH_RateHelpersSelected#0014</v>
+        <v>USD_YC1YRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="74" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -11968,7 +11968,7 @@
       </c>
       <c r="E7" s="68">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>5.1060000000000003E-3</v>
+        <v>5.0860000000000002E-3</v>
       </c>
       <c r="F7" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -11976,14 +11976,14 @@
       </c>
       <c r="G7" s="78">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H7" s="79">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41967</v>
+        <v>41982</v>
       </c>
       <c r="I7" s="64">
-        <v>0.99736884125987235</v>
+        <v>0.99742128363697291</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -11992,7 +11992,7 @@
       </c>
       <c r="E8" s="68">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>5.1859999999999996E-3</v>
+        <v>5.176E-3</v>
       </c>
       <c r="F8" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -12000,14 +12000,14 @@
       </c>
       <c r="G8" s="78">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H8" s="79">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42058</v>
+        <v>42072</v>
       </c>
       <c r="I8" s="64">
-        <v>0.9960255206307036</v>
+        <v>0.99609021310155077</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -12024,14 +12024,14 @@
       </c>
       <c r="G9" s="78">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H9" s="79">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42146</v>
+        <v>42164</v>
       </c>
       <c r="I9" s="64">
-        <v>0.99460897072645826</v>
+        <v>0.99460897072647148</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -12040,7 +12040,7 @@
       </c>
       <c r="E10" s="68">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>5.4499999999999991E-3</v>
+        <v>5.4699999999999992E-3</v>
       </c>
       <c r="F10" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -12048,14 +12048,14 @@
       </c>
       <c r="G10" s="78">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41813</v>
+        <v>41829</v>
       </c>
       <c r="H10" s="79">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42178</v>
+        <v>42194</v>
       </c>
       <c r="I10" s="64">
-        <v>0.99405880255588741</v>
+        <v>0.99406826701870843</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -12064,7 +12064,7 @@
       </c>
       <c r="E11" s="68">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>5.6099999999999995E-3</v>
+        <v>5.7099999999999998E-3</v>
       </c>
       <c r="F11" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -12072,14 +12072,14 @@
       </c>
       <c r="G11" s="78">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41842</v>
+        <v>41862</v>
       </c>
       <c r="H11" s="79">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42207</v>
+        <v>42227</v>
       </c>
       <c r="I11" s="64">
-        <v>0.99349479814171138</v>
+        <v>0.99337029873916827</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -12088,7 +12088,7 @@
       </c>
       <c r="E12" s="68">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>5.8200000000000005E-3</v>
+        <v>5.9699999999999996E-3</v>
       </c>
       <c r="F12" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -12096,14 +12096,14 @@
       </c>
       <c r="G12" s="78">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41873</v>
+        <v>41891</v>
       </c>
       <c r="H12" s="79">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42240</v>
+        <v>42256</v>
       </c>
       <c r="I12" s="64">
-        <v>0.99281648382454568</v>
+        <v>0.99270591025581445</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -12112,7 +12112,7 @@
       </c>
       <c r="E13" s="68">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>6.0799999999999995E-3</v>
+        <v>6.2700000000000004E-3</v>
       </c>
       <c r="F13" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -12120,14 +12120,14 @@
       </c>
       <c r="G13" s="78">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41904</v>
+        <v>41921</v>
       </c>
       <c r="H13" s="79">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42269</v>
+        <v>42286</v>
       </c>
       <c r="I13" s="64">
-        <v>0.99215263280371591</v>
+        <v>0.99198338751235837</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -12136,7 +12136,7 @@
       </c>
       <c r="E14" s="68">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>6.3899999999999998E-3</v>
+        <v>6.6400000000000001E-3</v>
       </c>
       <c r="F14" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -12144,14 +12144,14 @@
       </c>
       <c r="G14" s="78">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41934</v>
+        <v>41953</v>
       </c>
       <c r="H14" s="79">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42299</v>
+        <v>42318</v>
       </c>
       <c r="I14" s="64">
-        <v>0.9914199502182226</v>
+        <v>0.9911648221988224</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -12160,7 +12160,7 @@
       </c>
       <c r="E15" s="68">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>6.7799999999999996E-3</v>
+        <v>7.0500000000000007E-3</v>
       </c>
       <c r="F15" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -12168,14 +12168,14 @@
       </c>
       <c r="G15" s="78">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41967</v>
+        <v>41982</v>
       </c>
       <c r="H15" s="79">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42332</v>
+        <v>42347</v>
       </c>
       <c r="I15" s="64">
-        <v>0.990559569684619</v>
+        <v>0.99034239869961738</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -12184,7 +12184,7 @@
       </c>
       <c r="E16" s="68">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>8.2199999999999999E-3</v>
+        <v>8.6199999999999992E-3</v>
       </c>
       <c r="F16" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -12192,14 +12192,14 @@
       </c>
       <c r="G16" s="78">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>42058</v>
+        <v>42072</v>
       </c>
       <c r="H16" s="79">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>42423</v>
+        <v>42438</v>
       </c>
       <c r="I16" s="64">
-        <v>0.98779308839979829</v>
+        <v>0.98743664746868431</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
@@ -12208,7 +12208,7 @@
       </c>
       <c r="E17" s="68">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>7.754693010562118E-3</v>
+        <v>7.9799585295124899E-3</v>
       </c>
       <c r="F17" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -12216,14 +12216,14 @@
       </c>
       <c r="G17" s="78">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H17" s="79">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42513</v>
+        <v>42530</v>
       </c>
       <c r="I17" s="64">
-        <v>0.98440885222753161</v>
+        <v>0.9839806787945764</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.2">
@@ -12232,7 +12232,7 @@
       </c>
       <c r="E18" s="68">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.164901613355118E-2</v>
+        <v>1.2019217681891072E-2</v>
       </c>
       <c r="F18" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -12240,14 +12240,14 @@
       </c>
       <c r="G18" s="78">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H18" s="79">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42877</v>
+        <v>42895</v>
       </c>
       <c r="I18" s="64">
-        <v>0.96525878253079789</v>
+        <v>0.96417192346326674</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.2">
@@ -12256,7 +12256,7 @@
       </c>
       <c r="E19" s="68">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.5532928591970138E-2</v>
+        <v>1.6133293309975427E-2</v>
       </c>
       <c r="F19" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -12264,14 +12264,14 @@
       </c>
       <c r="G19" s="78">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H19" s="79">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>43242</v>
+        <v>43262</v>
       </c>
       <c r="I19" s="64">
-        <v>0.93897709264128637</v>
+        <v>0.93659667633381216</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.2">
@@ -12280,7 +12280,7 @@
       </c>
       <c r="E20" s="68">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.8856057589906713E-2</v>
+        <v>1.9626592515768052E-2</v>
       </c>
       <c r="F20" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -12288,14 +12288,14 @@
       </c>
       <c r="G20" s="78">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H20" s="79">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>43607</v>
+        <v>43626</v>
       </c>
       <c r="I20" s="64">
-        <v>0.9086696953706439</v>
+        <v>0.9050315423114208</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.2">
@@ -12304,7 +12304,7 @@
       </c>
       <c r="E21" s="68">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>2.1648616902011295E-2</v>
+        <v>2.2489103454696721E-2</v>
       </c>
       <c r="F21" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -12312,14 +12312,14 @@
       </c>
       <c r="G21" s="78">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H21" s="79">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43973</v>
+        <v>43991</v>
       </c>
       <c r="I21" s="64">
-        <v>0.87601100968173373</v>
+        <v>0.87145880704358913</v>
       </c>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.2">
@@ -12328,7 +12328,7 @@
       </c>
       <c r="E22" s="68">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>2.3930540650813428E-2</v>
+        <v>2.4811040117459097E-2</v>
       </c>
       <c r="F22" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -12336,14 +12336,14 @@
       </c>
       <c r="G22" s="78">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H22" s="79">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>44340</v>
+        <v>44356</v>
       </c>
       <c r="I22" s="64">
-        <v>0.84255463035943445</v>
+        <v>0.83729213356445997</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.2">
@@ -12352,7 +12352,7 @@
       </c>
       <c r="E23" s="68">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>2.5801991147985238E-2</v>
+        <v>2.6682497469501069E-2</v>
       </c>
       <c r="F23" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -12360,14 +12360,14 @@
       </c>
       <c r="G23" s="78">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H23" s="79">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>44704</v>
+        <v>44721</v>
       </c>
       <c r="I23" s="64">
-        <v>0.80930963518802534</v>
+        <v>0.80346357473916685</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.2">
@@ -12376,7 +12376,7 @@
       </c>
       <c r="E24" s="68">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>2.7353168245615473E-2</v>
+        <v>2.8223635133069854E-2</v>
       </c>
       <c r="F24" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -12384,14 +12384,14 @@
       </c>
       <c r="G24" s="78">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H24" s="79">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>45068</v>
+        <v>45086</v>
       </c>
       <c r="I24" s="64">
-        <v>0.77655994743449752</v>
+        <v>0.7702617551050962</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.2">
@@ -12400,7 +12400,7 @@
       </c>
       <c r="E25" s="68">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.8664063485976134E-2</v>
+        <v>2.9524682111459762E-2</v>
       </c>
       <c r="F25" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -12408,14 +12408,14 @@
       </c>
       <c r="G25" s="78">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H25" s="79">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>45434</v>
+        <v>45453</v>
       </c>
       <c r="I25" s="64">
-        <v>0.74436817887312723</v>
+        <v>0.73766550690825206</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.2">
@@ -12424,7 +12424,7 @@
       </c>
       <c r="E26" s="68">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>3.0715617484556201E-2</v>
+        <v>3.1586118645384104E-2</v>
       </c>
       <c r="F26" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -12432,14 +12432,14 @@
       </c>
       <c r="G26" s="78">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H26" s="79">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>46164</v>
+        <v>46182</v>
       </c>
       <c r="I26" s="64">
-        <v>0.68302041908465339</v>
+        <v>0.67558137748410629</v>
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.2">
@@ -12448,7 +12448,7 @@
       </c>
       <c r="E27" s="68">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>3.273691034385539E-2</v>
+        <v>3.3647436284933101E-2</v>
       </c>
       <c r="F27" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -12456,14 +12456,14 @@
       </c>
       <c r="G27" s="78">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H27" s="79">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>47260</v>
+        <v>47280</v>
       </c>
       <c r="I27" s="64">
-        <v>0.60028304790193754</v>
+        <v>0.5915357139288604</v>
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.2">
@@ -12472,7 +12472,7 @@
       </c>
       <c r="E28" s="68">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>3.452808326448225E-2</v>
+        <v>3.5448540914528488E-2</v>
       </c>
       <c r="F28" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -12480,14 +12480,14 @@
       </c>
       <c r="G28" s="78">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H28" s="79">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>49086</v>
+        <v>49104</v>
       </c>
       <c r="I28" s="64">
-        <v>0.48649997962345187</v>
+        <v>0.47703880368464735</v>
       </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.2">
@@ -12496,7 +12496,7 @@
       </c>
       <c r="E29" s="68">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>3.5348449501041962E-2</v>
+        <v>3.6238855439511539E-2</v>
       </c>
       <c r="F29" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -12504,14 +12504,14 @@
       </c>
       <c r="G29" s="78">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H29" s="79">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>50913</v>
+        <v>50930</v>
       </c>
       <c r="I29" s="64">
-        <v>0.39753262502199632</v>
+        <v>0.38838793736282945</v>
       </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.2">
@@ -12520,7 +12520,7 @@
       </c>
       <c r="E30" s="68">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>3.5728530220437316E-2</v>
+        <v>3.6599057160298439E-2</v>
       </c>
       <c r="F30" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -12528,14 +12528,14 @@
       </c>
       <c r="G30" s="78">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H30" s="79">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>52740</v>
+        <v>52757</v>
       </c>
       <c r="I30" s="64">
-        <v>0.32726536260446204</v>
+        <v>0.31856559327900347</v>
       </c>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.2">
@@ -12544,7 +12544,7 @@
       </c>
       <c r="E31" s="68">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>3.5886758472093862E-2</v>
+        <v>3.6771807077715532E-2</v>
       </c>
       <c r="F31" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -12552,14 +12552,14 @@
       </c>
       <c r="G31" s="78">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H31" s="79">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>54567</v>
+        <v>54583</v>
       </c>
       <c r="I31" s="64">
-        <v>0.27122092767378975</v>
+        <v>0.26262148272488151</v>
       </c>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.2">
@@ -12568,7 +12568,7 @@
       </c>
       <c r="E32" s="68">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>3.5898674654738019E-2</v>
+        <v>3.67991537539194E-2</v>
       </c>
       <c r="F32" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -12576,14 +12576,14 @@
       </c>
       <c r="G32" s="78">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H32" s="79">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>56391</v>
+        <v>56409</v>
       </c>
       <c r="I32" s="64">
-        <v>0.22667454825160219</v>
+        <v>0.21822969373208423</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
@@ -12592,7 +12592,7 @@
       </c>
       <c r="E33" s="68">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>3.572849704733444E-2</v>
+        <v>3.659896924229504E-2</v>
       </c>
       <c r="F33" s="68">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -12600,14 +12600,14 @@
       </c>
       <c r="G33" s="78">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41781</v>
+        <v>41799</v>
       </c>
       <c r="H33" s="79">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>60044</v>
+        <v>60062</v>
       </c>
       <c r="I33" s="64">
-        <v>0.16148492931212496</v>
+        <v>0.15470296919705304</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
@@ -15495,7 +15495,7 @@
       </c>
       <c r="C3" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B3,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005d4#0002</v>
+        <v>obj_005aa#0002</v>
       </c>
       <c r="D3" s="141" t="str">
         <f>Currency&amp;B3&amp;"D_SYNTH"&amp;$D$1&amp;QuoteSuffix</f>
@@ -15523,7 +15523,7 @@
       </c>
       <c r="C4" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B4,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005c5#0002</v>
+        <v>obj_005bf#0002</v>
       </c>
       <c r="D4" s="141" t="str">
         <f t="shared" ref="D4:D18" si="1">Currency&amp;B4&amp;"D_SYNTH"&amp;$D$1&amp;QuoteSuffix</f>
@@ -15551,7 +15551,7 @@
       </c>
       <c r="C5" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B5,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005b7#0002</v>
+        <v>obj_005c3#0002</v>
       </c>
       <c r="D5" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15579,7 +15579,7 @@
       </c>
       <c r="C6" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B6,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005ab#0002</v>
+        <v>obj_005ad#0002</v>
       </c>
       <c r="D6" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15607,7 +15607,7 @@
       </c>
       <c r="C7" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B7,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005bf#0002</v>
+        <v>obj_005dc#0002</v>
       </c>
       <c r="D7" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="C8" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B8,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005be#0002</v>
+        <v>obj_005d9#0002</v>
       </c>
       <c r="D8" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15663,7 +15663,7 @@
       </c>
       <c r="C9" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B9,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005c4#0002</v>
+        <v>obj_005a9#0002</v>
       </c>
       <c r="D9" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15691,7 +15691,7 @@
       </c>
       <c r="C10" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B10,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005d6#0002</v>
+        <v>obj_005c4#0002</v>
       </c>
       <c r="D10" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15719,7 +15719,7 @@
       </c>
       <c r="C11" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B11,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005dc#0002</v>
+        <v>obj_005ba#0002</v>
       </c>
       <c r="D11" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15747,7 +15747,7 @@
       </c>
       <c r="C12" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B12,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005cd#0002</v>
+        <v>obj_005db#0002</v>
       </c>
       <c r="D12" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15775,7 +15775,7 @@
       </c>
       <c r="C13" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B13,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005dd#0002</v>
+        <v>obj_005bb#0002</v>
       </c>
       <c r="D13" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15803,7 +15803,7 @@
       </c>
       <c r="C14" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B14,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005b6#0002</v>
+        <v>obj_005c2#0002</v>
       </c>
       <c r="D14" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15831,7 +15831,7 @@
       </c>
       <c r="C15" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B15,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005d0#0002</v>
+        <v>obj_005cc#0002</v>
       </c>
       <c r="D15" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15859,7 +15859,7 @@
       </c>
       <c r="C16" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B16,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005ca#0002</v>
+        <v>obj_005cf#0002</v>
       </c>
       <c r="D16" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15887,7 +15887,7 @@
       </c>
       <c r="C17" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B17,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005d8#0002</v>
+        <v>obj_005af#0002</v>
       </c>
       <c r="D17" s="141" t="str">
         <f t="shared" si="1"/>
@@ -15915,7 +15915,7 @@
       </c>
       <c r="C18" s="140" t="str">
         <f>_xll.qlLibor(,"USD",B18,,,Trigger,ObjectOverwrite)</f>
-        <v>obj_005c6#0002</v>
+        <v>obj_005ab#0002</v>
       </c>
       <c r="D18" s="141" t="str">
         <f t="shared" si="1"/>

</xml_diff>